<commit_message>
fixed incorrect figure sizing
</commit_message>
<xml_diff>
--- a/output/ecoinvent_electricity_comparison.xlsx
+++ b/output/ecoinvent_electricity_comparison.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="51">
   <si>
     <t>name_0</t>
   </si>
@@ -119,33 +119,30 @@
     <t>electricity production</t>
   </si>
   <si>
+    <t xml:space="preserve"> natural gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hard coal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nuclear</t>
+  </si>
+  <si>
     <t xml:space="preserve"> photovoltaic</t>
   </si>
   <si>
-    <t xml:space="preserve"> hydro</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> wind</t>
+    <t xml:space="preserve"> conventional power plant</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> boiling water reactor</t>
   </si>
   <si>
     <t xml:space="preserve"> 3kWp slanted-roof installation</t>
   </si>
   <si>
-    <t xml:space="preserve"> reservoir</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1-3MW turbine</t>
-  </si>
-  <si>
     <t xml:space="preserve"> multi-Si</t>
   </si>
   <si>
-    <t xml:space="preserve"> alpine region</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> onshore</t>
-  </si>
-  <si>
     <t xml:space="preserve"> panel</t>
   </si>
   <si>
@@ -155,19 +152,19 @@
     <t>kilowatt hour</t>
   </si>
   <si>
-    <t>IN-KA</t>
-  </si>
-  <si>
-    <t>IN-RJ</t>
-  </si>
-  <si>
-    <t>CN-BJ</t>
-  </si>
-  <si>
-    <t>CN-HB</t>
-  </si>
-  <si>
-    <t>PT</t>
+    <t>CN-JS</t>
+  </si>
+  <si>
+    <t>RoW</t>
+  </si>
+  <si>
+    <t>US-NPCC</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>IN-JH</t>
   </si>
   <si>
     <t>SUM</t>
@@ -731,79 +728,79 @@
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
         <v>44</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>45</v>
       </c>
-      <c r="I5" t="s">
-        <v>46</v>
-      </c>
       <c r="J5">
-        <v>0.0002609195365269829</v>
+        <v>5.286919471991329e-05</v>
       </c>
       <c r="K5">
-        <v>0.05607629913940771</v>
+        <v>0.5881428265178578</v>
       </c>
       <c r="L5">
-        <v>0.0001272224702508546</v>
+        <v>1.545157547629209e-05</v>
       </c>
       <c r="M5">
-        <v>0.05646444114618555</v>
+        <v>0.588211147288054</v>
       </c>
       <c r="N5">
-        <v>0.0004096740248563348</v>
+        <v>0.000644634679182998</v>
       </c>
       <c r="O5">
-        <v>0.06404512040555524</v>
+        <v>0.2170721411134519</v>
       </c>
       <c r="P5">
-        <v>5.200957810563865e-05</v>
+        <v>7.907773686730527e-06</v>
       </c>
       <c r="Q5">
-        <v>7.266580531066468e-05</v>
+        <v>0.0001796024813569905</v>
       </c>
       <c r="R5">
-        <v>0.0006660951589964609</v>
+        <v>0.001934277467896381</v>
       </c>
       <c r="S5">
-        <v>1.576156520834355e-09</v>
+        <v>1.142198550058577e-09</v>
       </c>
       <c r="T5">
-        <v>0.006591104696974544</v>
+        <v>0.0013688076167618</v>
       </c>
       <c r="U5">
-        <v>1.947786819588726e-08</v>
+        <v>1.202923719665467e-08</v>
       </c>
       <c r="V5">
-        <v>6.316699519801202e-09</v>
+        <v>5.099299971441437e-08</v>
       </c>
       <c r="W5">
-        <v>0.0002263699542517231</v>
+        <v>0.0007178805218160317</v>
       </c>
       <c r="X5">
-        <v>3.496668331453305e-09</v>
+        <v>1.659245295147601e-09</v>
       </c>
       <c r="Y5">
-        <v>0.0806349240756063</v>
+        <v>0.04455877808499443</v>
       </c>
       <c r="Z5">
-        <v>0.8637546785323285</v>
+        <v>9.281378319154575</v>
       </c>
       <c r="AA5">
-        <v>0.4259828439010588</v>
+        <v>0.170847548610212</v>
       </c>
       <c r="AB5">
-        <v>2.47044955455851e-06</v>
+        <v>1.040911988865314e-07</v>
       </c>
     </row>
     <row r="6" spans="1:28">
@@ -817,10 +814,10 @@
         <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -829,67 +826,67 @@
         <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J6">
-        <v>0.0004804631261999025</v>
+        <v>0.0001616986535232125</v>
       </c>
       <c r="K6">
-        <v>0.006484052851051176</v>
+        <v>1.053454477686903</v>
       </c>
       <c r="L6">
-        <v>3.730301560940804e-06</v>
+        <v>7.82396072599958e-05</v>
       </c>
       <c r="M6">
-        <v>0.006968246278812019</v>
+        <v>1.053694415947686</v>
       </c>
       <c r="N6">
-        <v>2.814286932433842e-05</v>
+        <v>0.01085113640346352</v>
       </c>
       <c r="O6">
-        <v>0.006420059515596608</v>
+        <v>0.07422882058379243</v>
       </c>
       <c r="P6">
-        <v>1.746552004442456e-06</v>
+        <v>0.0007531669661793517</v>
       </c>
       <c r="Q6">
-        <v>7.588468586616145e-06</v>
+        <v>0.001527883603109032</v>
       </c>
       <c r="R6">
-        <v>8.360493777727705e-05</v>
+        <v>0.01553304952034168</v>
       </c>
       <c r="S6">
-        <v>4.186395693542945e-10</v>
+        <v>1.561706663738776e-09</v>
       </c>
       <c r="T6">
-        <v>0.0004082124114318258</v>
+        <v>0.004843650936140326</v>
       </c>
       <c r="U6">
-        <v>1.001933090056153e-09</v>
+        <v>4.135860669938857e-08</v>
       </c>
       <c r="V6">
-        <v>4.608831990810072e-10</v>
+        <v>6.8087920470168e-09</v>
       </c>
       <c r="W6">
-        <v>2.366760076733885e-05</v>
+        <v>0.004120163950660458</v>
       </c>
       <c r="X6">
-        <v>5.214178563630209e-10</v>
+        <v>1.34248713786235e-08</v>
       </c>
       <c r="Y6">
-        <v>1.256094249416411</v>
+        <v>0.07718037347407579</v>
       </c>
       <c r="Z6">
-        <v>0.06146986362186379</v>
+        <v>15.35046263144623</v>
       </c>
       <c r="AA6">
-        <v>-0.2006223068534055</v>
+        <v>2.357584899634859</v>
       </c>
       <c r="AB6">
-        <v>2.247062283741605e-08</v>
+        <v>1.142804968737993e-07</v>
       </c>
     </row>
     <row r="7" spans="1:28">
@@ -900,82 +897,82 @@
         <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" t="s">
         <v>44</v>
       </c>
-      <c r="H7" t="s">
-        <v>45</v>
-      </c>
       <c r="I7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J7">
-        <v>0.0003627356893005789</v>
+        <v>2.624625341258119e-05</v>
       </c>
       <c r="K7">
-        <v>0.07795842079436487</v>
+        <v>0.01267051627996468</v>
       </c>
       <c r="L7">
-        <v>0.0001768672865817323</v>
+        <v>2.951349671891123e-05</v>
       </c>
       <c r="M7">
-        <v>0.07849802377024717</v>
+        <v>0.01272627603009617</v>
       </c>
       <c r="N7">
-        <v>0.0005695372288898008</v>
+        <v>7.404590847023137e-05</v>
       </c>
       <c r="O7">
-        <v>0.08903683950183613</v>
+        <v>0.02522830566466985</v>
       </c>
       <c r="P7">
-        <v>7.230478183316355e-05</v>
+        <v>8.869033765887167e-06</v>
       </c>
       <c r="Q7">
-        <v>0.0001010214924009057</v>
+        <v>5.99860802417057e-05</v>
       </c>
       <c r="R7">
-        <v>0.0009260191469645991</v>
+        <v>0.0001871872915509936</v>
       </c>
       <c r="S7">
-        <v>2.191205111126022e-09</v>
+        <v>5.676047713594472e-10</v>
       </c>
       <c r="T7">
-        <v>0.009163088886975304</v>
+        <v>1.184924149684349</v>
       </c>
       <c r="U7">
-        <v>2.707853171961306e-08</v>
+        <v>3.716515067226953e-09</v>
       </c>
       <c r="V7">
-        <v>8.781605183543211e-09</v>
+        <v>5.734081644121022e-08</v>
       </c>
       <c r="W7">
-        <v>0.0003147041516574072</v>
+        <v>5.125497889075731e-05</v>
       </c>
       <c r="X7">
-        <v>4.861140006467336e-09</v>
+        <v>2.871031731584624e-09</v>
       </c>
       <c r="Y7">
-        <v>0.1121003247045101</v>
+        <v>0.132818818140007</v>
       </c>
       <c r="Z7">
-        <v>1.200809463633813</v>
+        <v>14.25516923004214</v>
       </c>
       <c r="AA7">
-        <v>0.5922100835058547</v>
+        <v>0.0842862583437976</v>
       </c>
       <c r="AB7">
-        <v>3.434469622313611e-06</v>
+        <v>5.122173123339639e-08</v>
       </c>
     </row>
     <row r="8" spans="1:28">
@@ -986,82 +983,82 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
         <v>43</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>44</v>
       </c>
-      <c r="H8" t="s">
-        <v>45</v>
-      </c>
       <c r="I8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J8">
-        <v>0.0003627356893005789</v>
+        <v>0.0003627325464398601</v>
       </c>
       <c r="K8">
-        <v>0.07795842079436487</v>
+        <v>0.07795664333540409</v>
       </c>
       <c r="L8">
-        <v>0.0001768672865817323</v>
+        <v>0.0001768657828741938</v>
       </c>
       <c r="M8">
-        <v>0.07849802377024717</v>
+        <v>0.07849624166471814</v>
       </c>
       <c r="N8">
-        <v>0.0005695372288898008</v>
+        <v>0.0005695293100380925</v>
       </c>
       <c r="O8">
-        <v>0.08903683950183613</v>
+        <v>0.08903599101351864</v>
       </c>
       <c r="P8">
-        <v>7.230478183316355e-05</v>
+        <v>7.230455327629451e-05</v>
       </c>
       <c r="Q8">
-        <v>0.0001010214924009057</v>
+        <v>0.0001010197919175701</v>
       </c>
       <c r="R8">
-        <v>0.0009260191469645991</v>
+        <v>0.0009260025680486097</v>
       </c>
       <c r="S8">
-        <v>2.191205111126022e-09</v>
+        <v>2.191182268009862e-09</v>
       </c>
       <c r="T8">
-        <v>0.009163088886975304</v>
+        <v>0.009163412530311145</v>
       </c>
       <c r="U8">
-        <v>2.707853171961306e-08</v>
+        <v>2.707839544830219e-08</v>
       </c>
       <c r="V8">
-        <v>8.781605183543211e-09</v>
+        <v>8.781046048747718e-09</v>
       </c>
       <c r="W8">
-        <v>0.0003147041516574072</v>
+        <v>0.0003146990953766684</v>
       </c>
       <c r="X8">
-        <v>4.861140006467336e-09</v>
+        <v>4.861032952104225e-09</v>
       </c>
       <c r="Y8">
-        <v>0.1121003247045101</v>
+        <v>0.1121000975513579</v>
       </c>
       <c r="Z8">
-        <v>1.200809463633813</v>
+        <v>1.200792614502978</v>
       </c>
       <c r="AA8">
-        <v>0.5922100835058547</v>
+        <v>0.5922132848053911</v>
       </c>
       <c r="AB8">
-        <v>3.434469622313611e-06</v>
+        <v>3.43446632134495e-06</v>
       </c>
     </row>
     <row r="9" spans="1:28">
@@ -1072,82 +1069,82 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
         <v>42</v>
       </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
       <c r="G9" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="H9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J9">
-        <v>1.901853147557775e-05</v>
+        <v>0.0002866161599215045</v>
       </c>
       <c r="K9">
-        <v>0.01355435125351188</v>
+        <v>0.06159896547387024</v>
       </c>
       <c r="L9">
-        <v>1.125650154284683e-05</v>
+        <v>0.0001397519571148735</v>
       </c>
       <c r="M9">
-        <v>0.0135846262865303</v>
+        <v>0.06202533359090662</v>
       </c>
       <c r="N9">
-        <v>8.267983898582537e-05</v>
+        <v>0.0004500207128494442</v>
       </c>
       <c r="O9">
-        <v>0.03481528866340308</v>
+        <v>0.07035259496730721</v>
       </c>
       <c r="P9">
-        <v>9.864782724122685e-06</v>
+        <v>5.713173399827861e-05</v>
       </c>
       <c r="Q9">
-        <v>1.677694002034151e-05</v>
+        <v>7.982228679657696e-05</v>
       </c>
       <c r="R9">
-        <v>0.0001651697811778397</v>
+        <v>0.0007316954458659341</v>
       </c>
       <c r="S9">
-        <v>2.092410074240161e-09</v>
+        <v>1.731384071307037e-09</v>
       </c>
       <c r="T9">
-        <v>0.0009759227057396574</v>
+        <v>0.007240228704367536</v>
       </c>
       <c r="U9">
-        <v>6.284831605690913e-09</v>
+        <v>2.139614327108067e-08</v>
       </c>
       <c r="V9">
-        <v>1.153203030406501e-09</v>
+        <v>6.938798772388854e-09</v>
       </c>
       <c r="W9">
-        <v>5.836742340050394e-05</v>
+        <v>0.0002486639669571065</v>
       </c>
       <c r="X9">
-        <v>1.104786028901073e-09</v>
+        <v>3.841037214086325e-09</v>
       </c>
       <c r="Y9">
-        <v>0.004952693471708225</v>
+        <v>0.08857624308882502</v>
       </c>
       <c r="Z9">
-        <v>0.1902874890056038</v>
+        <v>0.9488214350334616</v>
       </c>
       <c r="AA9">
-        <v>0.3285667017201818</v>
+        <v>0.4679357036154478</v>
       </c>
       <c r="AB9">
-        <v>3.038103419993014e-07</v>
+        <v>2.713751427108127e-06</v>
       </c>
     </row>
   </sheetData>
@@ -1218,7 +1215,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:29">
@@ -1373,13 +1370,13 @@
         <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -1388,19 +1385,19 @@
         <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I5" t="s">
         <v>47</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>0.08711699836901678</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -1412,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>0.001289833240354371</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -1424,25 +1421,25 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5">
         <v>0</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5">
         <v>0</v>
       </c>
       <c r="X5">
-        <v>0</v>
+        <v>0.1029937912219481</v>
       </c>
       <c r="Y5">
         <v>1</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>0.9239466261889019</v>
       </c>
       <c r="AA5">
         <v>0</v>
@@ -1451,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="AC5">
-        <v>2</v>
+        <v>4.115347249020221</v>
       </c>
     </row>
     <row r="6" spans="1:29">
@@ -1462,13 +1459,13 @@
         <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -1477,70 +1474,70 @@
         <v>9</v>
       </c>
       <c r="H6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" t="s">
         <v>45</v>
       </c>
-      <c r="I6" t="s">
-        <v>50</v>
-      </c>
       <c r="J6">
-        <v>0</v>
+        <v>0.0791204333104106</v>
       </c>
       <c r="K6">
-        <v>0.09892075447338201</v>
+        <v>0.5529219622677178</v>
       </c>
       <c r="L6">
-        <v>0.04346962597854079</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>0.09249826072100553</v>
+        <v>0.5528362004465545</v>
       </c>
       <c r="N6">
-        <v>0.1007342775149334</v>
+        <v>0.05294460234678785</v>
       </c>
       <c r="O6">
-        <v>0.3436980859401192</v>
+        <v>1</v>
       </c>
       <c r="P6">
-        <v>0.1150571767373855</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>0.09834286699303087</v>
+        <v>0.08148825054328823</v>
       </c>
       <c r="R6">
-        <v>0.09682272985310678</v>
+        <v>0.1138476385554691</v>
       </c>
       <c r="S6">
-        <v>0.9442643814529346</v>
+        <v>0.3539059760834137</v>
       </c>
       <c r="T6">
-        <v>0.06484503760775102</v>
+        <v>0</v>
       </c>
       <c r="U6">
-        <v>0.2025915492539269</v>
+        <v>0.2208358188662738</v>
       </c>
       <c r="V6">
-        <v>0.08320429797057333</v>
+        <v>0.8743803201455498</v>
       </c>
       <c r="W6">
-        <v>0.1192284011305235</v>
+        <v>0.1638339779902565</v>
       </c>
       <c r="X6">
-        <v>0.1344252356165313</v>
+        <v>0</v>
       </c>
       <c r="Y6">
         <v>0</v>
       </c>
       <c r="Z6">
-        <v>0.1130634144397237</v>
+        <v>0.5785838412775223</v>
       </c>
       <c r="AA6">
-        <v>0.6674664342784901</v>
+        <v>0.03807739497757064</v>
       </c>
       <c r="AB6">
-        <v>0.08245597938483459</v>
+        <v>0.0156268535262453</v>
       </c>
       <c r="AC6">
-        <v>3.401088509346793</v>
+        <v>4.678403270337061</v>
       </c>
     </row>
     <row r="7" spans="1:29">
@@ -1551,85 +1548,85 @@
         <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s">
         <v>43</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>44</v>
       </c>
-      <c r="H7" t="s">
-        <v>45</v>
-      </c>
       <c r="I7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J7">
-        <v>0.5242254602547054</v>
+        <v>0.773790528483177</v>
       </c>
       <c r="K7">
-        <v>0.6938465874603905</v>
+        <v>0.04701114833453406</v>
       </c>
       <c r="L7">
-        <v>0.7132627882776404</v>
+        <v>0.770070885595398</v>
       </c>
       <c r="M7">
-        <v>0.6919662915671744</v>
+        <v>0.04735885342726558</v>
       </c>
       <c r="N7">
-        <v>0.7047194873589437</v>
+        <v>0.03488648485914445</v>
       </c>
       <c r="O7">
-        <v>0.6974982672957787</v>
+        <v>0.235213652797744</v>
       </c>
       <c r="P7">
-        <v>0.7123623455861753</v>
+        <v>0.06604945072453494</v>
       </c>
       <c r="Q7">
-        <v>0.6965132248464774</v>
+        <v>0.01351334561565585</v>
       </c>
       <c r="R7">
-        <v>0.6914534618084289</v>
+        <v>0.03548240862565399</v>
       </c>
       <c r="S7">
-        <v>0.653017857000137</v>
+        <v>0.7167993534947181</v>
       </c>
       <c r="T7">
-        <v>0.7062226751930161</v>
+        <v>0.004960833582440496</v>
       </c>
       <c r="U7">
-        <v>0.7085255009021494</v>
+        <v>0.4696770938400284</v>
       </c>
       <c r="V7">
-        <v>0.7037630065822559</v>
+        <v>0.002572759095457743</v>
       </c>
       <c r="W7">
-        <v>0.6964841799576916</v>
+        <v>0.04851644247536204</v>
       </c>
       <c r="X7">
-        <v>0.6855854757933679</v>
+        <v>0.1854378087030079</v>
       </c>
       <c r="Y7">
-        <v>0.06049054181303447</v>
+        <v>0.4987247340517232</v>
       </c>
       <c r="Z7">
-        <v>0.7041665319998098</v>
+        <v>0</v>
       </c>
       <c r="AA7">
-        <v>0.7903374765888759</v>
+        <v>0.1687633284528628</v>
       </c>
       <c r="AB7">
-        <v>0.7174617964708971</v>
+        <v>0.7869752318991931</v>
       </c>
       <c r="AC7">
-        <v>12.55190295675695</v>
+        <v>4.905804344057902</v>
       </c>
     </row>
     <row r="8" spans="1:29">
@@ -1640,85 +1637,85 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
         <v>43</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>44</v>
-      </c>
-      <c r="H8" t="s">
-        <v>45</v>
       </c>
       <c r="I8" t="s">
         <v>48</v>
       </c>
       <c r="J8">
-        <v>0.744871999270777</v>
+        <v>1</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0.06272783735751</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>0.06318153564222315</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>0.04597561853990628</v>
       </c>
       <c r="O8">
-        <v>1</v>
+        <v>0.3326022188806999</v>
       </c>
       <c r="P8">
-        <v>1</v>
+        <v>0.08640856796972896</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>0.02795407106874258</v>
       </c>
       <c r="R8">
-        <v>1</v>
+        <v>0.04814426621864945</v>
       </c>
       <c r="S8">
         <v>1</v>
       </c>
       <c r="T8">
-        <v>1</v>
+        <v>0.006585754494532314</v>
       </c>
       <c r="U8">
-        <v>1</v>
+        <v>0.6206318344200278</v>
       </c>
       <c r="V8">
-        <v>1</v>
+        <v>0.03902978408989978</v>
       </c>
       <c r="W8">
-        <v>1</v>
+        <v>0.0647456402474717</v>
       </c>
       <c r="X8">
-        <v>1</v>
+        <v>0.2721306655710689</v>
       </c>
       <c r="Y8">
-        <v>0.08563989480143001</v>
+        <v>0.7652536688660563</v>
       </c>
       <c r="Z8">
-        <v>1</v>
+        <v>0.0174960045201153</v>
       </c>
       <c r="AA8">
-        <v>1</v>
+        <v>0.2234317204241716</v>
       </c>
       <c r="AB8">
         <v>1</v>
       </c>
       <c r="AC8">
-        <v>17.83051189407221</v>
+        <v>6.676299188310804</v>
       </c>
     </row>
     <row r="9" spans="1:29">
@@ -1729,34 +1726,34 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
         <v>44</v>
       </c>
-      <c r="H9" t="s">
-        <v>45</v>
-      </c>
       <c r="I9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J9">
-        <v>0.744871999270777</v>
+        <v>0.4025495329750332</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0.3889870216252099</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -1765,7 +1762,7 @@
         <v>1</v>
       </c>
       <c r="O9">
-        <v>1</v>
+        <v>0.2554187618512486</v>
       </c>
       <c r="P9">
         <v>1</v>
@@ -1777,16 +1774,16 @@
         <v>1</v>
       </c>
       <c r="S9">
-        <v>1</v>
+        <v>0.6122910020804365</v>
       </c>
       <c r="T9">
-        <v>1</v>
+        <v>0.00293593649225411</v>
       </c>
       <c r="U9">
         <v>1</v>
       </c>
       <c r="V9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9">
         <v>1</v>
@@ -1795,7 +1792,7 @@
         <v>1</v>
       </c>
       <c r="Y9">
-        <v>0.08563989480143001</v>
+        <v>0.3696077564518244</v>
       </c>
       <c r="Z9">
         <v>1</v>
@@ -1804,10 +1801,10 @@
         <v>1</v>
       </c>
       <c r="AB9">
-        <v>1</v>
+        <v>0.01863854769019928</v>
       </c>
       <c r="AC9">
-        <v>17.83051189407221</v>
+        <v>13.05042855916621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>